<commit_message>
fixed dates, added ggplot function
</commit_message>
<xml_diff>
--- a/Date_State.xlsx
+++ b/Date_State.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emil\Desktop\UNI\DataVisualization\R_opgaver\Project\DataVis-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140AFB76-CE0F-44F2-AAA8-E6637A45B7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83425B9E-5C6C-4A4D-AD31-1E046267B2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{61B9E034-1CB9-4307-A4F5-CE0D06CF1F6F}"/>
   </bookViews>
@@ -27642,7 +27642,7 @@
   <dimension ref="A1:B5178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5178"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>